<commit_message>
CHANGED: Cards - Revised card list for next playtesting session.
</commit_message>
<xml_diff>
--- a/Documents/Card Lists/Card List - 01 Premiere.xlsx
+++ b/Documents/Card Lists/Card List - 01 Premiere.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="191">
   <si>
     <t>Card List - Premiere</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Oshiro Asteroid Belt</t>
   </si>
   <si>
-    <t>Pitiva Nebula</t>
-  </si>
-  <si>
     <t>Rahra Asteroid Belt</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>Collateral Damage</t>
   </si>
   <si>
-    <t>Each player draws one battle destiny. If that destiny draw exceeds 3, damage that player's flagships.</t>
-  </si>
-  <si>
     <t>End Of The Line</t>
   </si>
   <si>
@@ -358,9 +352,6 @@
     <t>Assault Cruiser</t>
   </si>
   <si>
-    <t>Namen retten!</t>
-  </si>
-  <si>
     <t>Assault Frigate</t>
   </si>
   <si>
@@ -373,9 +364,6 @@
     <t>UNIQUE. Bane is power +1 for each other attacking starship.</t>
   </si>
   <si>
-    <t>Karte vergessen?</t>
-  </si>
-  <si>
     <t>Cataclysm</t>
   </si>
   <si>
@@ -493,15 +481,9 @@
     <t>Interdictor</t>
   </si>
   <si>
-    <t>FLAGSHIP. ATTACK: Overload Artemis twice to make all enemy ships threat +1 this turn.</t>
-  </si>
-  <si>
     <t>Ares</t>
   </si>
   <si>
-    <t>FLAGSHIP. JUMP: Overload Hermes to draw an additional location card to pick from.</t>
-  </si>
-  <si>
     <t>FLAGSHIP. UPKEEP (1). Power +1 for each card in hand.</t>
   </si>
   <si>
@@ -596,13 +578,22 @@
   </si>
   <si>
     <t>Cruiser</t>
+  </si>
+  <si>
+    <t>Each player draws one battle destiny. If that destiny draw exceeds 3, damage that player's flagship.</t>
+  </si>
+  <si>
+    <t>FLAGSHIP. CLOAKING. ATTACK: Overload Artemis twice to make all enemy ships threat +1 this turn.</t>
+  </si>
+  <si>
+    <t>FLAGSHIP. CLOAKING. JUMP: Overload Ares to draw an additional location card to pick from.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +609,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -627,7 +626,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -644,18 +643,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -963,7 +972,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:N86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -986,59 +995,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s">
-        <v>109</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="I4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1056,6 +1068,9 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -1073,6 +1088,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -1090,6 +1108,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1104,6 +1125,9 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1121,6 +1145,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -1138,6 +1165,9 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -1155,6 +1185,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
@@ -1169,6 +1202,9 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
@@ -1179,13 +1215,16 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -1196,13 +1235,16 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -1213,13 +1255,16 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -1230,13 +1275,16 @@
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -1247,13 +1295,16 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -1264,13 +1315,16 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -1281,13 +1335,16 @@
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
@@ -1298,13 +1355,16 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
       <c r="B21" t="s">
         <v>37</v>
       </c>
@@ -1315,13 +1375,16 @@
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
@@ -1329,13 +1392,19 @@
         <v>29</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="K22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>19</v>
+      </c>
       <c r="B23" t="s">
         <v>39</v>
       </c>
@@ -1343,7 +1412,7 @@
         <v>29</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" t="s">
         <v>46</v>
@@ -1352,7 +1421,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20</v>
+      </c>
       <c r="B24" t="s">
         <v>40</v>
       </c>
@@ -1363,13 +1435,16 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>21</v>
+      </c>
       <c r="B25" t="s">
         <v>41</v>
       </c>
@@ -1377,16 +1452,19 @@
         <v>29</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>22</v>
+      </c>
       <c r="B26" t="s">
         <v>42</v>
       </c>
@@ -1394,284 +1472,335 @@
         <v>29</v>
       </c>
       <c r="H26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>23</v>
+      </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="K27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="K30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+      <c r="K31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="K32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>29</v>
       </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="I27" t="s">
-        <v>46</v>
-      </c>
-      <c r="K27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" t="s">
         <v>63</v>
       </c>
-      <c r="D28" t="s">
-        <v>64</v>
-      </c>
-      <c r="K28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
         <v>63</v>
-      </c>
-      <c r="D29" t="s">
-        <v>64</v>
-      </c>
-      <c r="K29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" t="s">
-        <v>64</v>
-      </c>
-      <c r="K30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" t="s">
-        <v>64</v>
-      </c>
-      <c r="K31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" t="s">
-        <v>64</v>
-      </c>
-      <c r="K32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" t="s">
-        <v>64</v>
-      </c>
-      <c r="K33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" t="s">
-        <v>64</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="K34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>31</v>
+      </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36">
         <v>0</v>
       </c>
-      <c r="K35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
       <c r="K36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>33</v>
+      </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>34</v>
+      </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>35</v>
+      </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="F39">
+        <v>8</v>
+      </c>
+      <c r="J39" t="s">
+        <v>108</v>
       </c>
       <c r="K39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>36</v>
+      </c>
       <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" t="s">
         <v>89</v>
       </c>
-      <c r="C40" t="s">
-        <v>90</v>
-      </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F40">
         <v>8</v>
       </c>
       <c r="J40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>37</v>
+      </c>
       <c r="B41" t="s">
         <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
-      </c>
-      <c r="F41">
-        <v>8</v>
-      </c>
-      <c r="J41" t="s">
-        <v>110</v>
+        <v>93</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>38</v>
+      </c>
       <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" t="s">
         <v>93</v>
-      </c>
-      <c r="C42" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" t="s">
-        <v>94</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>39</v>
+      </c>
       <c r="B43" t="s">
         <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1680,15 +1809,18 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>40</v>
+      </c>
       <c r="B44" t="s">
         <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1697,15 +1829,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>41</v>
+      </c>
       <c r="B45" t="s">
         <v>100</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1714,15 +1849,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>42</v>
+      </c>
       <c r="B46" t="s">
         <v>102</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1731,15 +1869,18 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>43</v>
+      </c>
       <c r="B47" t="s">
         <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1748,75 +1889,90 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>44</v>
+      </c>
       <c r="B48" t="s">
         <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>14</v>
+      </c>
+      <c r="J48" t="s">
+        <v>109</v>
       </c>
       <c r="K48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>45</v>
+      </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F49">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J49" t="s">
         <v>111</v>
       </c>
-      <c r="K49" t="s">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="C50" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" t="s">
+        <v>93</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>8</v>
+      </c>
+      <c r="J50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>47</v>
+      </c>
+      <c r="B51" t="s">
         <v>113</v>
       </c>
-      <c r="C50" t="s">
-        <v>90</v>
-      </c>
-      <c r="D50" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50">
-        <v>3</v>
-      </c>
-      <c r="F50">
-        <v>10</v>
-      </c>
-      <c r="J50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>115</v>
-      </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E51">
         <v>2</v>
@@ -1825,84 +1981,99 @@
         <v>8</v>
       </c>
       <c r="J51" t="s">
+        <v>114</v>
+      </c>
+      <c r="K51" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>48</v>
+      </c>
       <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <v>12</v>
+      </c>
+      <c r="J52" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
         <v>116</v>
       </c>
-      <c r="C52" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" t="s">
-        <v>94</v>
-      </c>
-      <c r="E52">
+      <c r="C53" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <v>10</v>
+      </c>
+      <c r="J53" t="s">
+        <v>112</v>
+      </c>
+      <c r="K53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54">
         <v>2</v>
       </c>
-      <c r="F52">
+      <c r="F54">
         <v>8</v>
       </c>
-      <c r="J52" t="s">
-        <v>117</v>
-      </c>
-      <c r="K52" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" t="s">
-        <v>90</v>
-      </c>
-      <c r="D53" t="s">
-        <v>94</v>
-      </c>
-      <c r="E53">
-        <v>4</v>
-      </c>
-      <c r="F53">
-        <v>13</v>
-      </c>
-      <c r="J53" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="J54" t="s">
+        <v>114</v>
+      </c>
+      <c r="K54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>51</v>
+      </c>
+      <c r="B55" t="s">
         <v>120</v>
       </c>
-      <c r="C54" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" t="s">
-        <v>94</v>
-      </c>
-      <c r="E54">
-        <v>3</v>
-      </c>
-      <c r="F54">
-        <v>10</v>
-      </c>
-      <c r="J54" t="s">
-        <v>115</v>
-      </c>
-      <c r="K54" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>122</v>
-      </c>
       <c r="C55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -1911,531 +2082,630 @@
         <v>8</v>
       </c>
       <c r="J55" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>52</v>
+      </c>
+      <c r="B56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56">
+        <v>12</v>
+      </c>
+      <c r="J56" t="s">
+        <v>111</v>
+      </c>
+      <c r="K56" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>53</v>
+      </c>
+      <c r="B57" t="s">
         <v>124</v>
       </c>
-      <c r="C56" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" t="s">
-        <v>94</v>
-      </c>
-      <c r="E56">
-        <v>2</v>
-      </c>
-      <c r="F56">
-        <v>8</v>
-      </c>
-      <c r="J56" t="s">
-        <v>117</v>
-      </c>
-      <c r="K56" t="s">
+      <c r="C57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" t="s">
+        <v>93</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>14</v>
+      </c>
+      <c r="J57" t="s">
+        <v>109</v>
+      </c>
+      <c r="K57" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>54</v>
+      </c>
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" t="s">
+        <v>93</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>6</v>
+      </c>
+      <c r="J58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>55</v>
+      </c>
+      <c r="B59" t="s">
         <v>126</v>
       </c>
-      <c r="C57" t="s">
-        <v>90</v>
-      </c>
-      <c r="D57" t="s">
-        <v>94</v>
-      </c>
-      <c r="E57">
-        <v>4</v>
-      </c>
-      <c r="F57">
-        <v>12</v>
-      </c>
-      <c r="J57" t="s">
-        <v>113</v>
-      </c>
-      <c r="K57" t="s">
+      <c r="C59" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="K59" t="s">
         <v>128</v>
       </c>
-      <c r="C58" t="s">
-        <v>90</v>
-      </c>
-      <c r="D58" t="s">
-        <v>94</v>
-      </c>
-      <c r="E58">
-        <v>5</v>
-      </c>
-      <c r="F58">
-        <v>14</v>
-      </c>
-      <c r="J58" t="s">
-        <v>111</v>
-      </c>
-      <c r="K58" t="s">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>56</v>
+      </c>
+      <c r="B60" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" t="s">
-        <v>90</v>
-      </c>
-      <c r="D59" t="s">
-        <v>94</v>
-      </c>
-      <c r="E59">
+      <c r="C60" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" t="s">
+        <v>127</v>
+      </c>
+      <c r="K60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>57</v>
+      </c>
+      <c r="B61" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" t="s">
+        <v>127</v>
+      </c>
+      <c r="K61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>58</v>
+      </c>
+      <c r="B62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" t="s">
+        <v>127</v>
+      </c>
+      <c r="K62" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>59</v>
+      </c>
+      <c r="B63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63" t="s">
+        <v>127</v>
+      </c>
+      <c r="K63" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" t="s">
+        <v>62</v>
+      </c>
+      <c r="D64" t="s">
+        <v>127</v>
+      </c>
+      <c r="K64" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>61</v>
+      </c>
+      <c r="B65" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65">
         <v>1</v>
       </c>
-      <c r="F59">
-        <v>6</v>
-      </c>
-      <c r="J59" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>130</v>
-      </c>
-      <c r="C60" t="s">
-        <v>63</v>
-      </c>
-      <c r="D60" t="s">
-        <v>131</v>
-      </c>
-      <c r="K60" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>133</v>
-      </c>
-      <c r="C61" t="s">
-        <v>63</v>
-      </c>
-      <c r="D61" t="s">
-        <v>131</v>
-      </c>
-      <c r="K61" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" t="s">
-        <v>63</v>
-      </c>
-      <c r="D62" t="s">
-        <v>131</v>
-      </c>
-      <c r="K62" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" t="s">
-        <v>63</v>
-      </c>
-      <c r="D63" t="s">
-        <v>131</v>
-      </c>
-      <c r="K63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>139</v>
-      </c>
-      <c r="C64" t="s">
-        <v>63</v>
-      </c>
-      <c r="D64" t="s">
-        <v>131</v>
-      </c>
-      <c r="K64" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+      <c r="K65" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>62</v>
+      </c>
+      <c r="B66" t="s">
         <v>141</v>
       </c>
-      <c r="C65" t="s">
-        <v>63</v>
-      </c>
-      <c r="D65" t="s">
-        <v>131</v>
-      </c>
-      <c r="K65" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>143</v>
-      </c>
       <c r="C66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D66" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="K66" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>63</v>
+      </c>
       <c r="B67" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" t="s">
+        <v>127</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="K67" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>64</v>
+      </c>
+      <c r="B68" t="s">
         <v>145</v>
       </c>
-      <c r="C67" t="s">
-        <v>77</v>
-      </c>
-      <c r="D67" t="s">
-        <v>131</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="K67" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>147</v>
-      </c>
       <c r="C68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D68" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="K68" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>65</v>
+      </c>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D69" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="K69" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>66</v>
+      </c>
+      <c r="B70" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" t="s">
+        <v>127</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="K70" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>67</v>
+      </c>
+      <c r="B71" t="s">
         <v>151</v>
       </c>
-      <c r="C70" t="s">
-        <v>77</v>
-      </c>
-      <c r="D70" t="s">
-        <v>131</v>
-      </c>
-      <c r="E70">
+      <c r="C71" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" t="s">
+        <v>127</v>
+      </c>
+      <c r="E71">
         <v>0</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K71" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>153</v>
-      </c>
-      <c r="C71" t="s">
-        <v>77</v>
-      </c>
-      <c r="D71" t="s">
-        <v>131</v>
-      </c>
-      <c r="E71">
-        <v>2</v>
-      </c>
-      <c r="K71" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>68</v>
+      </c>
       <c r="B72" t="s">
         <v>155</v>
       </c>
       <c r="C72" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D72" t="s">
-        <v>131</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
+        <v>127</v>
+      </c>
+      <c r="F72">
+        <v>8</v>
+      </c>
+      <c r="J72" t="s">
+        <v>154</v>
       </c>
       <c r="K72" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>69</v>
+      </c>
       <c r="B73" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D73" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F73">
         <v>8</v>
       </c>
       <c r="J73" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K73" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>70</v>
+      </c>
       <c r="B74" t="s">
         <v>157</v>
       </c>
       <c r="C74" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="D74" t="s">
-        <v>131</v>
-      </c>
-      <c r="F74">
-        <v>8</v>
-      </c>
-      <c r="J74" t="s">
         <v>158</v>
       </c>
       <c r="K74" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>71</v>
+      </c>
       <c r="B75" t="s">
+        <v>160</v>
+      </c>
+      <c r="C75" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" t="s">
+        <v>158</v>
+      </c>
+      <c r="K75" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>72</v>
+      </c>
+      <c r="B76" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" t="s">
+        <v>158</v>
+      </c>
+      <c r="K76" t="s">
         <v>163</v>
       </c>
-      <c r="C75" t="s">
-        <v>63</v>
-      </c>
-      <c r="D75" t="s">
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>73</v>
+      </c>
+      <c r="B77" t="s">
         <v>164</v>
       </c>
-      <c r="K75" t="s">
+      <c r="C77" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77" t="s">
+        <v>158</v>
+      </c>
+      <c r="K77" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>74</v>
+      </c>
+      <c r="B78" t="s">
         <v>166</v>
       </c>
-      <c r="C76" t="s">
-        <v>63</v>
-      </c>
-      <c r="K76" t="s">
+      <c r="C78" t="s">
+        <v>62</v>
+      </c>
+      <c r="D78" t="s">
+        <v>158</v>
+      </c>
+      <c r="K78" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>75</v>
+      </c>
+      <c r="B79" t="s">
         <v>168</v>
       </c>
-      <c r="C77" t="s">
-        <v>63</v>
-      </c>
-      <c r="K77" t="s">
+      <c r="C79" t="s">
+        <v>76</v>
+      </c>
+      <c r="D79" t="s">
+        <v>158</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="K79" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>76</v>
+      </c>
+      <c r="B80" t="s">
         <v>170</v>
       </c>
-      <c r="C78" t="s">
-        <v>63</v>
-      </c>
-      <c r="K78" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>172</v>
-      </c>
-      <c r="C79" t="s">
-        <v>63</v>
-      </c>
-      <c r="K79" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>174</v>
-      </c>
       <c r="C80" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="D80" t="s">
+        <v>158</v>
       </c>
       <c r="E80">
         <v>0</v>
       </c>
       <c r="K80" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>77</v>
+      </c>
       <c r="B81" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C81" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="D81" t="s">
+        <v>158</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="K81" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>78</v>
+      </c>
       <c r="B82" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C82" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="D82" t="s">
+        <v>158</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="K82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>79</v>
+      </c>
+      <c r="B83" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" t="s">
+        <v>89</v>
+      </c>
+      <c r="D83" t="s">
+        <v>158</v>
+      </c>
+      <c r="F83">
+        <v>8</v>
+      </c>
+      <c r="J83" t="s">
+        <v>185</v>
+      </c>
+      <c r="K83" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>80</v>
+      </c>
+      <c r="B84" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>180</v>
-      </c>
-      <c r="C83" t="s">
-        <v>77</v>
-      </c>
-      <c r="K83" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>182</v>
-      </c>
       <c r="C84" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="D84" t="s">
+        <v>158</v>
       </c>
       <c r="F84">
         <v>8</v>
       </c>
       <c r="J84" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="K84" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>81</v>
+      </c>
+      <c r="B85" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" t="s">
+        <v>89</v>
+      </c>
+      <c r="D85" t="s">
+        <v>158</v>
+      </c>
+      <c r="F85">
+        <v>9</v>
+      </c>
+      <c r="J85" t="s">
+        <v>177</v>
+      </c>
+      <c r="K85" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>82</v>
+      </c>
+      <c r="B86" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>185</v>
-      </c>
-      <c r="C85" t="s">
-        <v>90</v>
-      </c>
-      <c r="F85">
-        <v>6</v>
-      </c>
-      <c r="J85" t="s">
+      <c r="C86" t="s">
+        <v>89</v>
+      </c>
+      <c r="D86" t="s">
+        <v>158</v>
+      </c>
+      <c r="F86">
+        <v>8</v>
+      </c>
+      <c r="J86" t="s">
+        <v>187</v>
+      </c>
+      <c r="K86" t="s">
         <v>186</v>
-      </c>
-      <c r="K85" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>188</v>
-      </c>
-      <c r="C86" t="s">
-        <v>90</v>
-      </c>
-      <c r="F86">
-        <v>9</v>
-      </c>
-      <c r="J86" t="s">
-        <v>183</v>
-      </c>
-      <c r="K86" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>190</v>
-      </c>
-      <c r="C87" t="s">
-        <v>90</v>
-      </c>
-      <c r="F87">
-        <v>7</v>
-      </c>
-      <c r="J87" t="s">
-        <v>193</v>
-      </c>
-      <c r="K87" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2443,5 +2713,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CHANGED: Affiliations - Renamed Terran affiliation wings and enemy race.
</commit_message>
<xml_diff>
--- a/Documents/Card Lists/Card List - 01 Premiere.xlsx
+++ b/Documents/Card Lists/Card List - 01 Premiere.xlsx
@@ -295,9 +295,6 @@
     <t>A Change Of Plans</t>
   </si>
   <si>
-    <t>Enemy</t>
-  </si>
-  <si>
     <t>Any player may decide to shuffle his or her hand into the draw deck to discard all enemy ships, adding their threat again.</t>
   </si>
   <si>
@@ -490,9 +487,6 @@
     <t>Admiral Bright</t>
   </si>
   <si>
-    <t>Red Wing</t>
-  </si>
-  <si>
     <t>CAPTAIN of the Ardor. All ships fighting manned ship are power -2.</t>
   </si>
   <si>
@@ -587,6 +581,12 @@
   </si>
   <si>
     <t>FLAGSHIP. CLOAKING. JUMP: Overload Ares to draw an additional location card to pick from.</t>
+  </si>
+  <si>
+    <t>Green Wing</t>
+  </si>
+  <si>
+    <t>Dra'tar</t>
   </si>
 </sst>
 </file>
@@ -660,11 +660,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -995,55 +995,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1052,19 +1052,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5">
-        <v>-1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>-0.2</v>
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1072,19 +1069,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>-0.3</v>
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1092,19 +1086,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>-1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>-0.25</v>
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1112,16 +1103,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8">
-        <v>-1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>-0.35</v>
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1129,19 +1120,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>164</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9">
-        <v>-1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>-0.3</v>
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1149,19 +1137,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10">
-        <v>-1</v>
-      </c>
-      <c r="G10" s="1">
-        <v>-0.25</v>
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1169,19 +1157,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11">
         <v>0</v>
       </c>
-      <c r="G11" s="1">
-        <v>-0.25</v>
-      </c>
       <c r="K11" t="s">
-        <v>25</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1189,16 +1177,19 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12">
-        <v>-2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>-0.25</v>
+        <v>76</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1206,19 +1197,19 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="I13" t="s">
-        <v>44</v>
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1226,19 +1217,22 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
-        <v>45</v>
+        <v>89</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="J14" t="s">
+        <v>183</v>
       </c>
       <c r="K14" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1246,19 +1240,22 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>44</v>
+        <v>89</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="J15" t="s">
+        <v>178</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1266,19 +1263,22 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16" t="s">
-        <v>45</v>
+        <v>89</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>175</v>
       </c>
       <c r="K16" t="s">
-        <v>50</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1286,19 +1286,22 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>182</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>44</v>
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="J17" t="s">
+        <v>185</v>
       </c>
       <c r="K17" t="s">
-        <v>51</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1306,19 +1309,19 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>46</v>
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1326,19 +1329,19 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>53</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1346,19 +1349,19 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-      <c r="I20" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1366,19 +1369,19 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1386,19 +1389,19 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1406,19 +1409,19 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23" t="s">
-        <v>46</v>
+        <v>76</v>
+      </c>
+      <c r="D23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1426,19 +1429,19 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" t="s">
-        <v>46</v>
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1446,19 +1449,25 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="I25" t="s">
-        <v>45</v>
+        <v>89</v>
+      </c>
+      <c r="D25" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+      <c r="J25" t="s">
+        <v>108</v>
       </c>
       <c r="K25" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1466,19 +1475,22 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26">
         <v>3</v>
       </c>
-      <c r="I26" t="s">
-        <v>45</v>
-      </c>
-      <c r="K26" t="s">
-        <v>60</v>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="J26" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1486,16 +1498,22 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
-      </c>
-      <c r="K27" t="s">
-        <v>64</v>
+        <v>190</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="J27" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1503,16 +1521,25 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>190</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+      <c r="J28" t="s">
+        <v>113</v>
       </c>
       <c r="K28" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1520,16 +1547,22 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
-      </c>
-      <c r="K29" t="s">
-        <v>68</v>
+        <v>190</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>12</v>
+      </c>
+      <c r="J29" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1537,16 +1570,25 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>190</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="J30" t="s">
+        <v>111</v>
       </c>
       <c r="K30" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1554,16 +1596,25 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>190</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>8</v>
+      </c>
+      <c r="J31" t="s">
+        <v>113</v>
       </c>
       <c r="K31" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1571,16 +1622,25 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
+        <v>190</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+      <c r="J32" t="s">
+        <v>113</v>
       </c>
       <c r="K32" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1588,19 +1648,25 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D33" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>12</v>
+      </c>
+      <c r="J33" t="s">
+        <v>110</v>
       </c>
       <c r="K33" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1608,19 +1674,25 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>14</v>
+      </c>
+      <c r="J34" t="s">
+        <v>108</v>
       </c>
       <c r="K34" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1628,19 +1700,22 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="K35" t="s">
-        <v>81</v>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="J35" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1648,19 +1723,16 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="K36" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1668,19 +1740,16 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="K37" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1688,19 +1757,16 @@
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
+        <v>189</v>
       </c>
       <c r="K38" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1708,22 +1774,16 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
-      </c>
-      <c r="F39">
-        <v>8</v>
-      </c>
-      <c r="J39" t="s">
-        <v>108</v>
+        <v>189</v>
       </c>
       <c r="K39" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1731,22 +1791,16 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
-      </c>
-      <c r="F40">
-        <v>8</v>
-      </c>
-      <c r="J40" t="s">
-        <v>108</v>
+        <v>189</v>
       </c>
       <c r="K40" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1754,19 +1808,16 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="K41" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1774,19 +1825,19 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
         <v>76</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>188</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,19 +1845,19 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
         <v>76</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="K43" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -1814,19 +1865,19 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
         <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -1834,19 +1885,19 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C45" t="s">
         <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -1854,19 +1905,19 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
         <v>76</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K46" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -1874,19 +1925,19 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
         <v>76</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K47" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1894,25 +1945,22 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="C48" t="s">
         <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>93</v>
-      </c>
-      <c r="E48">
-        <v>5</v>
+        <v>189</v>
       </c>
       <c r="F48">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="J48" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K48" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -1920,22 +1968,22 @@
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
         <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="F49">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J49" t="s">
-        <v>111</v>
+        <v>107</v>
+      </c>
+      <c r="K49" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -1943,22 +1991,16 @@
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="C50" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D50" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50">
-        <v>2</v>
-      </c>
-      <c r="F50">
-        <v>8</v>
-      </c>
-      <c r="J50" t="s">
-        <v>112</v>
+        <v>126</v>
+      </c>
+      <c r="K50" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -1966,25 +2008,16 @@
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D51" t="s">
-        <v>93</v>
-      </c>
-      <c r="E51">
-        <v>2</v>
-      </c>
-      <c r="F51">
-        <v>8</v>
-      </c>
-      <c r="J51" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="K51" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -1992,22 +2025,16 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D52" t="s">
-        <v>93</v>
-      </c>
-      <c r="E52">
-        <v>4</v>
-      </c>
-      <c r="F52">
-        <v>12</v>
-      </c>
-      <c r="J52" t="s">
-        <v>109</v>
+        <v>126</v>
+      </c>
+      <c r="K52" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2015,25 +2042,16 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
-      </c>
-      <c r="E53">
-        <v>3</v>
-      </c>
-      <c r="F53">
-        <v>10</v>
-      </c>
-      <c r="J53" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="K53" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2041,25 +2059,16 @@
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D54" t="s">
-        <v>93</v>
-      </c>
-      <c r="E54">
-        <v>2</v>
-      </c>
-      <c r="F54">
-        <v>8</v>
-      </c>
-      <c r="J54" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="K54" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2067,25 +2076,16 @@
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D55" t="s">
-        <v>93</v>
-      </c>
-      <c r="E55">
-        <v>2</v>
-      </c>
-      <c r="F55">
-        <v>8</v>
-      </c>
-      <c r="J55" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="K55" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2093,25 +2093,19 @@
         <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D56" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="E56">
-        <v>4</v>
-      </c>
-      <c r="F56">
-        <v>12</v>
-      </c>
-      <c r="J56" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="K56" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -2119,25 +2113,19 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D57" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="E57">
-        <v>5</v>
-      </c>
-      <c r="F57">
-        <v>14</v>
-      </c>
-      <c r="J57" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="K57" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -2145,22 +2133,19 @@
         <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D58" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58">
-        <v>6</v>
-      </c>
-      <c r="J58" t="s">
-        <v>114</v>
+        <v>0</v>
+      </c>
+      <c r="K58" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -2168,16 +2153,19 @@
         <v>55</v>
       </c>
       <c r="B59" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" t="s">
         <v>126</v>
       </c>
-      <c r="C59" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" t="s">
-        <v>127</v>
+      <c r="E59">
+        <v>0</v>
       </c>
       <c r="K59" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2185,16 +2173,19 @@
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
       </c>
       <c r="K60" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2202,16 +2193,19 @@
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="C61" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D61" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
       </c>
       <c r="K61" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -2219,16 +2213,19 @@
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="C62" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D62" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
       </c>
       <c r="K62" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2236,16 +2233,22 @@
         <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C63" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D63" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="F63">
+        <v>8</v>
+      </c>
+      <c r="J63" t="s">
+        <v>153</v>
       </c>
       <c r="K63" t="s">
-        <v>136</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -2253,16 +2256,22 @@
         <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D64" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="F64">
+        <v>8</v>
+      </c>
+      <c r="J64" t="s">
+        <v>153</v>
       </c>
       <c r="K64" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -2270,19 +2279,19 @@
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" t="s">
-        <v>127</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="F65">
+        <v>-1</v>
+      </c>
+      <c r="G65" s="1">
+        <v>-0.2</v>
       </c>
       <c r="K65" t="s">
-        <v>144</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -2290,19 +2299,19 @@
         <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
-      </c>
-      <c r="D66" t="s">
-        <v>127</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
+        <v>-0.3</v>
       </c>
       <c r="K66" t="s">
-        <v>142</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -2310,19 +2319,19 @@
         <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
-      </c>
-      <c r="D67" t="s">
-        <v>127</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="F67">
+        <v>-1</v>
+      </c>
+      <c r="G67" s="1">
+        <v>-0.25</v>
       </c>
       <c r="K67" t="s">
-        <v>140</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -2330,19 +2339,16 @@
         <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>76</v>
-      </c>
-      <c r="D68" t="s">
-        <v>127</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="K68" t="s">
-        <v>146</v>
+        <v>16</v>
+      </c>
+      <c r="F68">
+        <v>-1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>-0.35</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -2350,19 +2356,19 @@
         <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="C69" t="s">
-        <v>76</v>
-      </c>
-      <c r="D69" t="s">
-        <v>127</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="F69">
+        <v>-1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>-0.3</v>
       </c>
       <c r="K69" t="s">
-        <v>148</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -2370,19 +2376,19 @@
         <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>149</v>
+        <v>22</v>
       </c>
       <c r="C70" t="s">
-        <v>76</v>
-      </c>
-      <c r="D70" t="s">
-        <v>127</v>
-      </c>
-      <c r="E70">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="F70">
+        <v>-1</v>
+      </c>
+      <c r="G70" s="1">
+        <v>-0.25</v>
       </c>
       <c r="K70" t="s">
-        <v>150</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -2390,19 +2396,19 @@
         <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>151</v>
+        <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>76</v>
-      </c>
-      <c r="D71" t="s">
-        <v>127</v>
-      </c>
-      <c r="E71">
+        <v>16</v>
+      </c>
+      <c r="F71">
         <v>0</v>
       </c>
+      <c r="G71" s="1">
+        <v>-0.25</v>
+      </c>
       <c r="K71" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -2410,22 +2416,16 @@
         <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>155</v>
+        <v>27</v>
       </c>
       <c r="C72" t="s">
-        <v>89</v>
-      </c>
-      <c r="D72" t="s">
-        <v>127</v>
+        <v>16</v>
       </c>
       <c r="F72">
-        <v>8</v>
-      </c>
-      <c r="J72" t="s">
-        <v>154</v>
-      </c>
-      <c r="K72" t="s">
-        <v>190</v>
+        <v>-2</v>
+      </c>
+      <c r="G72" s="1">
+        <v>-0.25</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -2433,22 +2433,19 @@
         <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>153</v>
+        <v>28</v>
       </c>
       <c r="C73" t="s">
-        <v>89</v>
-      </c>
-      <c r="D73" t="s">
-        <v>127</v>
-      </c>
-      <c r="F73">
-        <v>8</v>
-      </c>
-      <c r="J73" t="s">
-        <v>154</v>
+        <v>29</v>
+      </c>
+      <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73" t="s">
+        <v>44</v>
       </c>
       <c r="K73" t="s">
-        <v>189</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -2456,16 +2453,19 @@
         <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
-      </c>
-      <c r="D74" t="s">
-        <v>158</v>
+        <v>29</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>45</v>
       </c>
       <c r="K74" t="s">
-        <v>159</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -2473,16 +2473,19 @@
         <v>71</v>
       </c>
       <c r="B75" t="s">
-        <v>160</v>
+        <v>31</v>
       </c>
       <c r="C75" t="s">
-        <v>62</v>
-      </c>
-      <c r="D75" t="s">
-        <v>158</v>
+        <v>29</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75" t="s">
+        <v>44</v>
       </c>
       <c r="K75" t="s">
-        <v>161</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -2490,16 +2493,19 @@
         <v>72</v>
       </c>
       <c r="B76" t="s">
-        <v>162</v>
+        <v>32</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
-      </c>
-      <c r="D76" t="s">
-        <v>158</v>
+        <v>29</v>
+      </c>
+      <c r="H76">
+        <v>3</v>
+      </c>
+      <c r="I76" t="s">
+        <v>45</v>
       </c>
       <c r="K76" t="s">
-        <v>163</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -2507,16 +2513,19 @@
         <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>164</v>
+        <v>33</v>
       </c>
       <c r="C77" t="s">
-        <v>62</v>
-      </c>
-      <c r="D77" t="s">
-        <v>158</v>
+        <v>29</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77" t="s">
+        <v>44</v>
       </c>
       <c r="K77" t="s">
-        <v>165</v>
+        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -2524,16 +2533,19 @@
         <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
       <c r="C78" t="s">
-        <v>62</v>
-      </c>
-      <c r="D78" t="s">
-        <v>158</v>
+        <v>29</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78" t="s">
+        <v>46</v>
       </c>
       <c r="K78" t="s">
-        <v>167</v>
+        <v>52</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -2541,19 +2553,19 @@
         <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>168</v>
+        <v>35</v>
       </c>
       <c r="C79" t="s">
-        <v>76</v>
-      </c>
-      <c r="D79" t="s">
-        <v>158</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79" t="s">
+        <v>45</v>
       </c>
       <c r="K79" t="s">
-        <v>169</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -2561,19 +2573,19 @@
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="C80" t="s">
-        <v>76</v>
-      </c>
-      <c r="D80" t="s">
-        <v>158</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="H80">
+        <v>2</v>
+      </c>
+      <c r="I80" t="s">
+        <v>45</v>
       </c>
       <c r="K80" t="s">
-        <v>171</v>
+        <v>54</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -2581,19 +2593,19 @@
         <v>77</v>
       </c>
       <c r="B81" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
       <c r="C81" t="s">
-        <v>76</v>
-      </c>
-      <c r="D81" t="s">
-        <v>158</v>
-      </c>
-      <c r="E81">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="H81">
+        <v>2</v>
+      </c>
+      <c r="I81" t="s">
+        <v>45</v>
       </c>
       <c r="K81" t="s">
-        <v>173</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -2601,19 +2613,19 @@
         <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>174</v>
+        <v>38</v>
       </c>
       <c r="C82" t="s">
-        <v>76</v>
-      </c>
-      <c r="D82" t="s">
-        <v>158</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="H82">
+        <v>2</v>
+      </c>
+      <c r="I82" t="s">
+        <v>45</v>
       </c>
       <c r="K82" t="s">
-        <v>175</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -2621,22 +2633,19 @@
         <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>176</v>
+        <v>39</v>
       </c>
       <c r="C83" t="s">
-        <v>89</v>
-      </c>
-      <c r="D83" t="s">
-        <v>158</v>
-      </c>
-      <c r="F83">
-        <v>8</v>
-      </c>
-      <c r="J83" t="s">
-        <v>185</v>
+        <v>29</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83" t="s">
+        <v>46</v>
       </c>
       <c r="K83" t="s">
-        <v>178</v>
+        <v>57</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -2644,22 +2653,19 @@
         <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>179</v>
+        <v>40</v>
       </c>
       <c r="C84" t="s">
-        <v>89</v>
-      </c>
-      <c r="D84" t="s">
-        <v>158</v>
-      </c>
-      <c r="F84">
-        <v>8</v>
-      </c>
-      <c r="J84" t="s">
-        <v>180</v>
+        <v>29</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>46</v>
       </c>
       <c r="K84" t="s">
-        <v>181</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -2667,22 +2673,19 @@
         <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>182</v>
+        <v>41</v>
       </c>
       <c r="C85" t="s">
-        <v>89</v>
-      </c>
-      <c r="D85" t="s">
-        <v>158</v>
-      </c>
-      <c r="F85">
-        <v>9</v>
-      </c>
-      <c r="J85" t="s">
-        <v>177</v>
+        <v>29</v>
+      </c>
+      <c r="H85">
+        <v>2</v>
+      </c>
+      <c r="I85" t="s">
+        <v>45</v>
       </c>
       <c r="K85" t="s">
-        <v>183</v>
+        <v>59</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -2690,25 +2693,27 @@
         <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>184</v>
+        <v>42</v>
       </c>
       <c r="C86" t="s">
-        <v>89</v>
-      </c>
-      <c r="D86" t="s">
-        <v>158</v>
-      </c>
-      <c r="F86">
-        <v>8</v>
-      </c>
-      <c r="J86" t="s">
-        <v>187</v>
+        <v>29</v>
+      </c>
+      <c r="H86">
+        <v>3</v>
+      </c>
+      <c r="I86" t="s">
+        <v>45</v>
       </c>
       <c r="K86" t="s">
-        <v>186</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A5:N86">
+    <sortCondition ref="D5:D86"/>
+    <sortCondition ref="C5:C86"/>
+    <sortCondition ref="B5:B86"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>

</xml_diff>

<commit_message>
ADDED: Card List - Paper prototype column to design flow.
</commit_message>
<xml_diff>
--- a/Documents/Card Lists/Card List - 01 Premiere.xlsx
+++ b/Documents/Card Lists/Card List - 01 Premiere.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="192">
   <si>
     <t>Card List - Premiere</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>Dra'tar</t>
+  </si>
+  <si>
+    <t>PROTOTYPED</t>
   </si>
 </sst>
 </file>
@@ -972,7 +975,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N86"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -990,11 +993,12 @@
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1002,8 +1006,8 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1041,13 +1045,16 @@
         <v>8</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1064,7 +1071,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1081,7 +1088,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1115,7 +1122,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1132,7 +1139,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1152,7 +1159,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1172,7 +1179,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1192,7 +1199,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1235,7 +1242,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1258,7 +1265,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
CHANGED: Card List - Increased threat of player effects and power of non-unique enemy starships.
</commit_message>
<xml_diff>
--- a/Documents/Card Lists/Card List - 01 Premiere.xlsx
+++ b/Documents/Card Lists/Card List - 01 Premiere.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="192">
   <si>
     <t>Card List - Premiere</t>
   </si>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1153,7 @@
         <v>63</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="s">
         <v>167</v>
@@ -1173,7 +1173,7 @@
         <v>63</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="s">
         <v>169</v>
@@ -1193,7 +1193,7 @@
         <v>63</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="s">
         <v>171</v>
@@ -1213,7 +1213,7 @@
         <v>63</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="s">
         <v>173</v>
@@ -1494,7 +1494,7 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J26" t="s">
         <v>110</v>
@@ -1517,7 +1517,7 @@
         <v>2</v>
       </c>
       <c r="F27">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J27" t="s">
         <v>111</v>
@@ -1719,10 +1719,13 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J35" t="s">
         <v>113</v>
+      </c>
+      <c r="K35" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1841,7 +1844,7 @@
         <v>189</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" t="s">
         <v>77</v>
@@ -1861,7 +1864,7 @@
         <v>189</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" t="s">
         <v>79</v>
@@ -1901,7 +1904,7 @@
         <v>189</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" t="s">
         <v>83</v>
@@ -2169,7 +2172,7 @@
         <v>126</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" t="s">
         <v>145</v>
@@ -2189,7 +2192,7 @@
         <v>126</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K60" t="s">
         <v>147</v>
@@ -2229,7 +2232,7 @@
         <v>126</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K62" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
CHANGED: Card Lists - Added starship class abbreviations and changed Purple Wing starship names.
</commit_message>
<xml_diff>
--- a/Documents/Card Lists/Card List - 01 Premiere.xlsx
+++ b/Documents/Card Lists/Card List - 01 Premiere.xlsx
@@ -265,18 +265,12 @@
     <t>WRAP UP: If there are no enemy starships, repair a flagship.</t>
   </si>
   <si>
-    <t>Moscow</t>
-  </si>
-  <si>
     <t>Starship</t>
   </si>
   <si>
     <t>FLAGSHIP. Overload to draw a card.</t>
   </si>
   <si>
-    <t>Washington</t>
-  </si>
-  <si>
     <t>A Change Of Plans</t>
   </si>
   <si>
@@ -316,15 +310,9 @@
     <t>Player ships don't get any power bonuses from captains until end of turn.</t>
   </si>
   <si>
-    <t>Agony</t>
-  </si>
-  <si>
     <t>Starship Class</t>
   </si>
   <si>
-    <t>Dreadnought</t>
-  </si>
-  <si>
     <t>Behemoth</t>
   </si>
   <si>
@@ -337,42 +325,24 @@
     <t>Assault Frigate</t>
   </si>
   <si>
-    <t>Bane</t>
-  </si>
-  <si>
     <t>Swarm Frigate</t>
   </si>
   <si>
     <t>UNIQUE. Bane is power +1 for each other attacking starship.</t>
   </si>
   <si>
-    <t>Cataclysm</t>
-  </si>
-  <si>
     <t>UNIQUE. Each time a player loses a fight, add (1).</t>
   </si>
   <si>
-    <t>Curse</t>
-  </si>
-  <si>
     <t>UNIQUE. Draws one battle destiny.</t>
   </si>
   <si>
-    <t>Decay</t>
-  </si>
-  <si>
     <t>UNIQUE. Power +2 while fighting a damaged ship.</t>
   </si>
   <si>
-    <t>Disaster</t>
-  </si>
-  <si>
     <t>UNIQUE. Power +2 while the threat pool is empty.</t>
   </si>
   <si>
-    <t>Horror</t>
-  </si>
-  <si>
     <t>UNIQUE. Every time Horror wins a fight, damage the losing starship.</t>
   </si>
   <si>
@@ -439,15 +409,9 @@
     <t>FIGHT: Make a starship +2 (or +4 if there is at least one unassigned player ship).</t>
   </si>
   <si>
-    <t>Artemis</t>
-  </si>
-  <si>
     <t>Interdictor</t>
   </si>
   <si>
-    <t>Ares</t>
-  </si>
-  <si>
     <t>FLAGSHIP. UPKEEP (1). Power +1 for each card in hand.</t>
   </si>
   <si>
@@ -490,27 +454,15 @@
     <t>FIGHT: Overload a starship to make it power +4.</t>
   </si>
   <si>
-    <t>Ardor</t>
-  </si>
-  <si>
     <t>Battleship</t>
   </si>
   <si>
     <t>FLAGSHIP. UPKEEP (1). Power +x, where x is the number of locations on the table.</t>
   </si>
   <si>
-    <t>Faith</t>
-  </si>
-  <si>
-    <t>Justice</t>
-  </si>
-  <si>
     <t>FLAGSHIP. UPKEEP (1). Power +x, where x is the threat of the enemy ship the Justice is fighting.</t>
   </si>
   <si>
-    <t>Truth</t>
-  </si>
-  <si>
     <t>FLAGSHIP. Power +2 while at a space location.</t>
   </si>
   <si>
@@ -569,6 +521,54 @@
   </si>
   <si>
     <t>Ships can't cloak.</t>
+  </si>
+  <si>
+    <t>Frigate</t>
+  </si>
+  <si>
+    <t>DB Agony</t>
+  </si>
+  <si>
+    <t>TRB Ardor</t>
+  </si>
+  <si>
+    <t>TRB Faith</t>
+  </si>
+  <si>
+    <t>TRB Justice</t>
+  </si>
+  <si>
+    <t>TRB Truth</t>
+  </si>
+  <si>
+    <t>TRF Moscow</t>
+  </si>
+  <si>
+    <t>TRF Washington</t>
+  </si>
+  <si>
+    <t>DSF Bane</t>
+  </si>
+  <si>
+    <t>DAF Cataclysm</t>
+  </si>
+  <si>
+    <t>DSF Curse</t>
+  </si>
+  <si>
+    <t>DSF Decay</t>
+  </si>
+  <si>
+    <t>DAC Disaster</t>
+  </si>
+  <si>
+    <t>DB Horror</t>
+  </si>
+  <si>
+    <t>TRI Pegasus</t>
+  </si>
+  <si>
+    <t>TRI Golem</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1015,7 @@
         <v>43</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>7</v>
@@ -1024,7 +1024,7 @@
         <v>8</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>9</v>
@@ -1038,7 +1038,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
         <v>61</v>
@@ -1047,7 +1047,7 @@
         <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
         <v>61</v>
@@ -1064,7 +1064,7 @@
         <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>61</v>
@@ -1081,7 +1081,7 @@
         <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
@@ -1098,7 +1098,7 @@
         <v>62</v>
       </c>
       <c r="K8" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1106,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
         <v>61</v>
@@ -1115,7 +1115,7 @@
         <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C10" t="s">
         <v>72</v>
@@ -1135,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1143,7 +1143,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C11" t="s">
         <v>72</v>
@@ -1155,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
         <v>72</v>
@@ -1175,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
         <v>72</v>
@@ -1195,7 +1195,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1203,10 +1203,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
         <v>62</v>
@@ -1215,10 +1215,10 @@
         <v>8</v>
       </c>
       <c r="J14" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="K14" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1226,10 +1226,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
         <v>62</v>
@@ -1238,10 +1238,10 @@
         <v>8</v>
       </c>
       <c r="J15" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="K15" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1249,10 +1249,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
         <v>62</v>
@@ -1261,10 +1261,10 @@
         <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="K16" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1272,10 +1272,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
         <v>62</v>
@@ -1284,10 +1284,10 @@
         <v>8</v>
       </c>
       <c r="J17" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="K17" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1295,19 +1295,19 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
         <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1315,19 +1315,19 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1335,19 +1335,19 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
         <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1355,19 +1355,19 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
         <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1375,19 +1375,19 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
         <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1395,19 +1395,19 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
         <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1415,19 +1415,19 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
         <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1435,13 +1435,13 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -1450,10 +1450,10 @@
         <v>14</v>
       </c>
       <c r="J25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1461,13 +1461,13 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -1476,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1484,13 +1484,13 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D27" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1499,7 +1499,7 @@
         <v>9</v>
       </c>
       <c r="J27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1507,13 +1507,13 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -1522,10 +1522,10 @@
         <v>8</v>
       </c>
       <c r="J28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1533,13 +1533,13 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -1548,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="J29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1556,13 +1556,13 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>178</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -1571,10 +1571,10 @@
         <v>10</v>
       </c>
       <c r="J30" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K30" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1582,13 +1582,13 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -1597,10 +1597,10 @@
         <v>8</v>
       </c>
       <c r="J31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K31" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1608,13 +1608,13 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -1623,10 +1623,10 @@
         <v>8</v>
       </c>
       <c r="J32" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1634,13 +1634,13 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -1649,10 +1649,10 @@
         <v>12</v>
       </c>
       <c r="J33" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K33" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1660,13 +1660,13 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -1675,10 +1675,10 @@
         <v>14</v>
       </c>
       <c r="J34" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K34" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1686,13 +1686,13 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1701,10 +1701,10 @@
         <v>7</v>
       </c>
       <c r="J35" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1718,10 +1718,10 @@
         <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="K36" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1735,7 +1735,7 @@
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="K37" t="s">
         <v>64</v>
@@ -1752,10 +1752,10 @@
         <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="K38" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1769,7 +1769,7 @@
         <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="K39" t="s">
         <v>67</v>
@@ -1786,7 +1786,7 @@
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="K40" t="s">
         <v>69</v>
@@ -1803,10 +1803,10 @@
         <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="K41" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1820,7 +1820,7 @@
         <v>72</v>
       </c>
       <c r="D42" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1840,13 +1840,13 @@
         <v>72</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -1860,7 +1860,7 @@
         <v>72</v>
       </c>
       <c r="D44" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1880,7 +1880,7 @@
         <v>72</v>
       </c>
       <c r="D45" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1900,7 +1900,7 @@
         <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E46">
         <v>3</v>
@@ -1920,7 +1920,7 @@
         <v>72</v>
       </c>
       <c r="D47" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -1934,22 +1934,22 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" t="s">
         <v>83</v>
       </c>
-      <c r="C48" t="s">
-        <v>84</v>
-      </c>
       <c r="D48" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="F48">
         <v>8</v>
       </c>
       <c r="J48" t="s">
-        <v>102</v>
+        <v>169</v>
       </c>
       <c r="K48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -1957,22 +1957,22 @@
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D49" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="F49">
         <v>8</v>
       </c>
       <c r="J49" t="s">
-        <v>102</v>
+        <v>169</v>
       </c>
       <c r="K49" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -1980,16 +1980,16 @@
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K50" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -1997,16 +1997,16 @@
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
         <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K51" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2014,16 +2014,16 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C52" t="s">
         <v>61</v>
       </c>
       <c r="D52" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K52" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2031,16 +2031,16 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C53" t="s">
         <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K53" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2048,16 +2048,16 @@
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
         <v>61</v>
       </c>
       <c r="D54" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K54" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2065,19 +2065,19 @@
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C55" t="s">
         <v>72</v>
       </c>
       <c r="D55" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="K55" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2085,19 +2085,19 @@
         <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
         <v>72</v>
       </c>
       <c r="D56" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="K56" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -2105,19 +2105,19 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C57" t="s">
         <v>72</v>
       </c>
       <c r="D57" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="K57" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -2125,19 +2125,19 @@
         <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C58" t="s">
         <v>72</v>
       </c>
       <c r="D58" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="K58" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -2145,19 +2145,19 @@
         <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C59" t="s">
         <v>72</v>
       </c>
       <c r="D59" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E59">
         <v>2</v>
       </c>
       <c r="K59" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2165,19 +2165,19 @@
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C60" t="s">
         <v>72</v>
       </c>
       <c r="D60" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="K60" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2185,22 +2185,22 @@
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="C61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D61" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F61">
         <v>8</v>
       </c>
       <c r="J61" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="K61" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -2208,22 +2208,22 @@
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>141</v>
+        <v>184</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D62" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F62">
         <v>8</v>
       </c>
       <c r="J62" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="K62" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
         <v>45</v>
       </c>
       <c r="K72" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CHANGED: Card List - Reduced printed power of non-blue starships. Reduced power bonuses of non-blue Fight effects.
</commit_message>
<xml_diff>
--- a/Documents/Card Lists/Card List - 01 Premiere.xlsx
+++ b/Documents/Card Lists/Card List - 01 Premiere.xlsx
@@ -235,9 +235,6 @@
     <t>Effect</t>
   </si>
   <si>
-    <t>FIGHT: Make a starship power +3.</t>
-  </si>
-  <si>
     <t>Emergency Procedures</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>Never Say Die</t>
   </si>
   <si>
-    <t>FIGHT: Make a starship power +2 (or +4 if that starship is not damaged).</t>
-  </si>
-  <si>
     <t>Rise From The Ashes</t>
   </si>
   <si>
@@ -394,9 +388,6 @@
     <t>Surprise Assault</t>
   </si>
   <si>
-    <t>FIGHT: Make a starship power +2 (of +4 if it has CLOAKING).</t>
-  </si>
-  <si>
     <t>They Are Coming</t>
   </si>
   <si>
@@ -406,9 +397,6 @@
     <t>Watch Your Back</t>
   </si>
   <si>
-    <t>FIGHT: Make a starship +2 (or +4 if there is at least one unassigned player ship).</t>
-  </si>
-  <si>
     <t>Interdictor</t>
   </si>
   <si>
@@ -569,6 +557,18 @@
   </si>
   <si>
     <t>TRI Golem</t>
+  </si>
+  <si>
+    <t>FIGHT: Make a starship power +2 (or +3 if you have still two or more cards in hand after playing this one).</t>
+  </si>
+  <si>
+    <t>FIGHT: Make a starship power +2 (or +3 if that starship is not damaged).</t>
+  </si>
+  <si>
+    <t>FIGHT: Make a starship power +2 (of +3 if it has CLOAKING).</t>
+  </si>
+  <si>
+    <t>FIGHT: Make a starship +2 (or +3 if there is at least one unassigned player ship).</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1015,7 @@
         <v>43</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>7</v>
@@ -1024,7 +1024,7 @@
         <v>8</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>9</v>
@@ -1038,7 +1038,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
         <v>61</v>
@@ -1047,7 +1047,7 @@
         <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
         <v>61</v>
@@ -1064,7 +1064,7 @@
         <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
         <v>61</v>
@@ -1081,7 +1081,7 @@
         <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
@@ -1098,7 +1098,7 @@
         <v>62</v>
       </c>
       <c r="K8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1106,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
         <v>61</v>
@@ -1115,7 +1115,7 @@
         <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
         <v>72</v>
@@ -1135,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1143,7 +1143,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
         <v>72</v>
@@ -1155,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
         <v>72</v>
@@ -1175,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
         <v>72</v>
@@ -1195,7 +1195,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1203,10 +1203,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
         <v>62</v>
@@ -1215,10 +1215,10 @@
         <v>8</v>
       </c>
       <c r="J14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1226,10 +1226,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
         <v>62</v>
@@ -1238,10 +1238,10 @@
         <v>8</v>
       </c>
       <c r="J15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1249,10 +1249,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
         <v>62</v>
@@ -1261,10 +1261,10 @@
         <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1272,10 +1272,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
         <v>62</v>
@@ -1284,10 +1284,10 @@
         <v>8</v>
       </c>
       <c r="J17" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1295,19 +1295,19 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1315,19 +1315,19 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1335,19 +1335,19 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
         <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1355,19 +1355,19 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
         <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1375,19 +1375,19 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
         <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1395,19 +1395,19 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
         <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1415,19 +1415,19 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
         <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1435,13 +1435,13 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -1450,10 +1450,10 @@
         <v>14</v>
       </c>
       <c r="J25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1461,13 +1461,13 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -1476,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="J26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1484,13 +1484,13 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1499,7 +1499,7 @@
         <v>9</v>
       </c>
       <c r="J27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1507,13 +1507,13 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -1522,10 +1522,10 @@
         <v>8</v>
       </c>
       <c r="J28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1533,13 +1533,13 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -1548,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="J29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1556,13 +1556,13 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -1571,10 +1571,10 @@
         <v>10</v>
       </c>
       <c r="J30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1582,13 +1582,13 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -1597,10 +1597,10 @@
         <v>8</v>
       </c>
       <c r="J31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1608,13 +1608,13 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -1623,10 +1623,10 @@
         <v>8</v>
       </c>
       <c r="J32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1634,13 +1634,13 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -1649,10 +1649,10 @@
         <v>12</v>
       </c>
       <c r="J33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1660,13 +1660,13 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -1675,10 +1675,10 @@
         <v>14</v>
       </c>
       <c r="J34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1686,13 +1686,13 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D35" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1701,10 +1701,10 @@
         <v>7</v>
       </c>
       <c r="J35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1718,10 +1718,10 @@
         <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K36" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1735,7 +1735,7 @@
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K37" t="s">
         <v>64</v>
@@ -1752,10 +1752,10 @@
         <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K38" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1769,7 +1769,7 @@
         <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K39" t="s">
         <v>67</v>
@@ -1786,7 +1786,7 @@
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K40" t="s">
         <v>69</v>
@@ -1803,10 +1803,10 @@
         <v>61</v>
       </c>
       <c r="D41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K41" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1820,13 +1820,13 @@
         <v>72</v>
       </c>
       <c r="D42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="K42" t="s">
-        <v>73</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1834,19 +1834,19 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" t="s">
         <v>72</v>
       </c>
       <c r="D43" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -1854,19 +1854,19 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
         <v>72</v>
       </c>
       <c r="D44" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="K44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -1874,19 +1874,19 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" t="s">
         <v>72</v>
       </c>
       <c r="D45" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="K45" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -1894,19 +1894,19 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
         <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="K46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -1914,19 +1914,19 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
         <v>72</v>
       </c>
       <c r="D47" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E47">
         <v>2</v>
       </c>
       <c r="K47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1934,22 +1934,22 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F48">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J48" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -1957,22 +1957,22 @@
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F49">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J49" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K49" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -1980,16 +1980,16 @@
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K50" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -1997,16 +1997,16 @@
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C51" t="s">
         <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2014,16 +2014,16 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C52" t="s">
         <v>61</v>
       </c>
       <c r="D52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K52" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2031,16 +2031,16 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C53" t="s">
         <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K53" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2048,16 +2048,16 @@
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
         <v>61</v>
       </c>
       <c r="D54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2065,19 +2065,19 @@
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C55" t="s">
         <v>72</v>
       </c>
       <c r="D55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="K55" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2085,19 +2085,19 @@
         <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C56" t="s">
         <v>72</v>
       </c>
       <c r="D56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="K56" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -2105,19 +2105,19 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C57" t="s">
         <v>72</v>
       </c>
       <c r="D57" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="K57" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -2125,19 +2125,19 @@
         <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C58" t="s">
         <v>72</v>
       </c>
       <c r="D58" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="K58" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -2145,19 +2145,19 @@
         <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C59" t="s">
         <v>72</v>
       </c>
       <c r="D59" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E59">
         <v>2</v>
       </c>
       <c r="K59" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2165,19 +2165,19 @@
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C60" t="s">
         <v>72</v>
       </c>
       <c r="D60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="K60" t="s">
-        <v>130</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2185,22 +2185,22 @@
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D61" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F61">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J61" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K61" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -2208,22 +2208,22 @@
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D62" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F62">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J62" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K62" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
         <v>45</v>
       </c>
       <c r="K72" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ADDED: Cards - One new card per affiliation.
</commit_message>
<xml_diff>
--- a/Documents/Card Lists/Card List - 01 Premiere.xlsx
+++ b/Documents/Card Lists/Card List - 01 Premiere.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="190">
   <si>
     <t>Card List - Premiere</t>
   </si>
@@ -566,6 +566,24 @@
   </si>
   <si>
     <t>Unique enemy ships are threat -1.</t>
+  </si>
+  <si>
+    <t>Target Eliminated</t>
+  </si>
+  <si>
+    <t>FIGHT: Make a starship power +1. If that starship's power exceeds the enemy power, draw a card.</t>
+  </si>
+  <si>
+    <t>Good As New!</t>
+  </si>
+  <si>
+    <t>MAIN: Repair a starship that is damaged at least twice.</t>
+  </si>
+  <si>
+    <t>No Second Guessing</t>
+  </si>
+  <si>
+    <t>MAIN: If your discard pile contains more cards than your draw deck, draw two cards.</t>
   </si>
 </sst>
 </file>
@@ -656,10 +674,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -966,7 +984,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N84"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -989,12 +1007,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1057,7 +1075,7 @@
       <c r="K5" t="s">
         <v>147</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1075,7 +1093,7 @@
       <c r="K6" t="s">
         <v>148</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1093,7 +1111,7 @@
       <c r="K7" t="s">
         <v>181</v>
       </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1111,7 +1129,7 @@
       <c r="K8" t="s">
         <v>177</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1129,7 +1147,7 @@
       <c r="K9" t="s">
         <v>149</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1150,7 +1168,7 @@
       <c r="K10" t="s">
         <v>132</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1171,7 +1189,7 @@
       <c r="K11" t="s">
         <v>134</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1192,7 +1210,7 @@
       <c r="K12" t="s">
         <v>136</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1213,38 +1231,35 @@
       <c r="K13" t="s">
         <v>138</v>
       </c>
-      <c r="L13" s="5"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
         <v>61</v>
       </c>
-      <c r="F14">
-        <v>8</v>
-      </c>
-      <c r="J14" t="s">
-        <v>139</v>
+      <c r="E14">
+        <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>140</v>
-      </c>
-      <c r="L14" s="5"/>
+        <v>185</v>
+      </c>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
         <v>78</v>
@@ -1259,16 +1274,16 @@
         <v>139</v>
       </c>
       <c r="K15" t="s">
-        <v>150</v>
-      </c>
-      <c r="L15" s="5"/>
+        <v>140</v>
+      </c>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
         <v>78</v>
@@ -1283,16 +1298,16 @@
         <v>139</v>
       </c>
       <c r="K16" t="s">
-        <v>141</v>
-      </c>
-      <c r="L16" s="5"/>
+        <v>150</v>
+      </c>
+      <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
         <v>78</v>
@@ -1307,37 +1322,40 @@
         <v>139</v>
       </c>
       <c r="K17" t="s">
-        <v>142</v>
-      </c>
-      <c r="L17" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="J18" t="s">
+        <v>139</v>
       </c>
       <c r="K18" t="s">
-        <v>81</v>
-      </c>
-      <c r="L18" s="5"/>
+        <v>142</v>
+      </c>
+      <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
         <v>70</v>
@@ -1349,16 +1367,16 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>151</v>
-      </c>
-      <c r="L19" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
         <v>70</v>
@@ -1370,16 +1388,16 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>84</v>
-      </c>
-      <c r="L20" s="5"/>
+        <v>151</v>
+      </c>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
         <v>70</v>
@@ -1391,16 +1409,16 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>86</v>
-      </c>
-      <c r="L21" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
         <v>70</v>
@@ -1412,16 +1430,16 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>88</v>
-      </c>
-      <c r="L22" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
@@ -1433,16 +1451,16 @@
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>90</v>
-      </c>
-      <c r="L23" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
         <v>70</v>
@@ -1454,43 +1472,37 @@
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>92</v>
-      </c>
-      <c r="L24" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>146</v>
       </c>
       <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="F25">
-        <v>14</v>
-      </c>
-      <c r="J25" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>95</v>
-      </c>
-      <c r="L25" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="L25" s="4"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="C26" t="s">
         <v>78</v>
@@ -1499,22 +1511,25 @@
         <v>146</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J26" t="s">
-        <v>96</v>
-      </c>
-      <c r="L26" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="K26" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26" s="4"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
         <v>78</v>
@@ -1523,22 +1538,22 @@
         <v>146</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J27" t="s">
-        <v>97</v>
-      </c>
-      <c r="L27" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
         <v>78</v>
@@ -1550,22 +1565,19 @@
         <v>2</v>
       </c>
       <c r="F28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J28" t="s">
-        <v>98</v>
-      </c>
-      <c r="K28" t="s">
-        <v>99</v>
-      </c>
-      <c r="L28" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="L28" s="4"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>165</v>
       </c>
       <c r="C29" t="s">
         <v>78</v>
@@ -1574,22 +1586,25 @@
         <v>146</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F29">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J29" t="s">
-        <v>94</v>
-      </c>
-      <c r="L29" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="K29" t="s">
+        <v>99</v>
+      </c>
+      <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
         <v>78</v>
@@ -1598,25 +1613,22 @@
         <v>146</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J30" t="s">
-        <v>97</v>
-      </c>
-      <c r="K30" t="s">
-        <v>100</v>
-      </c>
-      <c r="L30" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="L30" s="4"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
         <v>78</v>
@@ -1625,25 +1637,25 @@
         <v>146</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K31" t="s">
-        <v>101</v>
-      </c>
-      <c r="L31" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" t="s">
         <v>78</v>
@@ -1661,16 +1673,16 @@
         <v>98</v>
       </c>
       <c r="K32" t="s">
-        <v>102</v>
-      </c>
-      <c r="L32" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C33" t="s">
         <v>78</v>
@@ -1679,25 +1691,25 @@
         <v>146</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F33">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J33" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K33" t="s">
-        <v>103</v>
-      </c>
-      <c r="L33" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C34" t="s">
         <v>78</v>
@@ -1706,25 +1718,25 @@
         <v>146</v>
       </c>
       <c r="E34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J34" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K34" t="s">
-        <v>104</v>
-      </c>
-      <c r="L34" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="C35" t="s">
         <v>78</v>
@@ -1733,43 +1745,52 @@
         <v>146</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F35">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J35" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="K35" t="s">
-        <v>90</v>
-      </c>
-      <c r="L35" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="J36" t="s">
+        <v>98</v>
       </c>
       <c r="K36" t="s">
-        <v>154</v>
-      </c>
-      <c r="L36" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
         <v>60</v>
@@ -1778,16 +1799,16 @@
         <v>145</v>
       </c>
       <c r="K37" t="s">
-        <v>63</v>
-      </c>
-      <c r="L37" s="5"/>
+        <v>154</v>
+      </c>
+      <c r="L37" s="4"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
         <v>60</v>
@@ -1796,16 +1817,16 @@
         <v>145</v>
       </c>
       <c r="K38" t="s">
-        <v>178</v>
-      </c>
-      <c r="L38" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
         <v>60</v>
@@ -1814,16 +1835,16 @@
         <v>145</v>
       </c>
       <c r="K39" t="s">
-        <v>66</v>
-      </c>
-      <c r="L39" s="5"/>
+        <v>178</v>
+      </c>
+      <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
         <v>60</v>
@@ -1832,16 +1853,16 @@
         <v>145</v>
       </c>
       <c r="K40" t="s">
-        <v>182</v>
-      </c>
-      <c r="L40" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
         <v>60</v>
@@ -1850,37 +1871,34 @@
         <v>145</v>
       </c>
       <c r="K41" t="s">
-        <v>152</v>
-      </c>
-      <c r="L41" s="5"/>
+        <v>182</v>
+      </c>
+      <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
         <v>145</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
       <c r="K42" t="s">
-        <v>173</v>
-      </c>
-      <c r="L42" s="5"/>
+        <v>152</v>
+      </c>
+      <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C43" t="s">
         <v>70</v>
@@ -1892,16 +1910,16 @@
         <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>153</v>
-      </c>
-      <c r="L43" s="5"/>
+        <v>173</v>
+      </c>
+      <c r="L43" s="4"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
         <v>70</v>
@@ -1913,16 +1931,16 @@
         <v>1</v>
       </c>
       <c r="K44" t="s">
-        <v>179</v>
-      </c>
-      <c r="L44" s="5"/>
+        <v>153</v>
+      </c>
+      <c r="L44" s="4"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="C45" t="s">
         <v>70</v>
@@ -1934,16 +1952,16 @@
         <v>1</v>
       </c>
       <c r="K45" t="s">
-        <v>174</v>
-      </c>
-      <c r="L45" s="5"/>
+        <v>187</v>
+      </c>
+      <c r="L45" s="4"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
         <v>70</v>
@@ -1952,19 +1970,19 @@
         <v>145</v>
       </c>
       <c r="E46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>75</v>
-      </c>
-      <c r="L46" s="5"/>
+        <v>179</v>
+      </c>
+      <c r="L46" s="4"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C47" t="s">
         <v>70</v>
@@ -1976,100 +1994,106 @@
         <v>1</v>
       </c>
       <c r="K47" t="s">
-        <v>77</v>
-      </c>
-      <c r="L47" s="5"/>
+        <v>174</v>
+      </c>
+      <c r="L47" s="4"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D48" t="s">
         <v>145</v>
       </c>
-      <c r="F48">
-        <v>7</v>
-      </c>
-      <c r="J48" t="s">
-        <v>157</v>
+      <c r="E48">
+        <v>3</v>
       </c>
       <c r="K48" t="s">
-        <v>79</v>
-      </c>
-      <c r="L48" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="L48" s="4"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
         <v>145</v>
       </c>
-      <c r="F49">
-        <v>7</v>
-      </c>
-      <c r="J49" t="s">
-        <v>157</v>
+      <c r="E49">
+        <v>1</v>
       </c>
       <c r="K49" t="s">
-        <v>125</v>
-      </c>
-      <c r="L49" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="L49" s="4"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>163</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D50" t="s">
-        <v>106</v>
+        <v>145</v>
+      </c>
+      <c r="F50">
+        <v>7</v>
+      </c>
+      <c r="J50" t="s">
+        <v>157</v>
       </c>
       <c r="K50" t="s">
-        <v>107</v>
-      </c>
-      <c r="L50" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="L50" s="4"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D51" t="s">
-        <v>106</v>
+        <v>145</v>
+      </c>
+      <c r="F51">
+        <v>7</v>
+      </c>
+      <c r="J51" t="s">
+        <v>157</v>
       </c>
       <c r="K51" t="s">
-        <v>109</v>
-      </c>
-      <c r="L51" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="L51" s="4"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
         <v>60</v>
@@ -2078,16 +2102,16 @@
         <v>106</v>
       </c>
       <c r="K52" t="s">
-        <v>180</v>
-      </c>
-      <c r="L52" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="L52" s="4"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
         <v>60</v>
@@ -2096,16 +2120,16 @@
         <v>106</v>
       </c>
       <c r="K53" t="s">
-        <v>112</v>
-      </c>
-      <c r="L53" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="L53" s="4"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C54" t="s">
         <v>60</v>
@@ -2114,58 +2138,52 @@
         <v>106</v>
       </c>
       <c r="K54" t="s">
-        <v>114</v>
-      </c>
-      <c r="L54" s="5"/>
+        <v>180</v>
+      </c>
+      <c r="L54" s="4"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D55" t="s">
         <v>106</v>
       </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
       <c r="K55" t="s">
-        <v>119</v>
-      </c>
-      <c r="L55" s="5"/>
+        <v>112</v>
+      </c>
+      <c r="L55" s="4"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D56" t="s">
         <v>106</v>
       </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
       <c r="K56" t="s">
-        <v>155</v>
-      </c>
-      <c r="L56" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="L56" s="4"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C57" t="s">
         <v>70</v>
@@ -2174,19 +2192,19 @@
         <v>106</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K57" t="s">
-        <v>116</v>
-      </c>
-      <c r="L57" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="L57" s="4"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
         <v>70</v>
@@ -2198,16 +2216,16 @@
         <v>1</v>
       </c>
       <c r="K58" t="s">
-        <v>175</v>
-      </c>
-      <c r="L58" s="5"/>
+        <v>155</v>
+      </c>
+      <c r="L58" s="4"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
         <v>70</v>
@@ -2216,19 +2234,19 @@
         <v>106</v>
       </c>
       <c r="E59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K59" t="s">
-        <v>122</v>
-      </c>
-      <c r="L59" s="5"/>
+        <v>116</v>
+      </c>
+      <c r="L59" s="4"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>188</v>
       </c>
       <c r="C60" t="s">
         <v>70</v>
@@ -2240,127 +2258,127 @@
         <v>1</v>
       </c>
       <c r="K60" t="s">
-        <v>176</v>
-      </c>
-      <c r="L60" s="5"/>
+        <v>189</v>
+      </c>
+      <c r="L60" s="4"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>171</v>
+        <v>120</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D61" t="s">
         <v>106</v>
       </c>
-      <c r="F61">
-        <v>7</v>
-      </c>
-      <c r="J61" t="s">
-        <v>124</v>
+      <c r="E61">
+        <v>1</v>
       </c>
       <c r="K61" t="s">
-        <v>144</v>
-      </c>
-      <c r="L61" s="5"/>
+        <v>175</v>
+      </c>
+      <c r="L61" s="4"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>172</v>
+        <v>121</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D62" t="s">
         <v>106</v>
       </c>
-      <c r="F62">
-        <v>7</v>
-      </c>
-      <c r="J62" t="s">
-        <v>124</v>
+      <c r="E62">
+        <v>2</v>
       </c>
       <c r="K62" t="s">
-        <v>143</v>
-      </c>
-      <c r="L62" s="5"/>
+        <v>122</v>
+      </c>
+      <c r="L62" s="4"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="C63" t="s">
-        <v>16</v>
-      </c>
-      <c r="F63">
-        <v>-1</v>
-      </c>
-      <c r="G63" s="1">
-        <v>-0.2</v>
+        <v>70</v>
+      </c>
+      <c r="D63" t="s">
+        <v>106</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
       </c>
       <c r="K63" t="s">
-        <v>13</v>
-      </c>
-      <c r="L63" s="5"/>
+        <v>176</v>
+      </c>
+      <c r="L63" s="4"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
       <c r="C64" t="s">
-        <v>16</v>
+        <v>78</v>
+      </c>
+      <c r="D64" t="s">
+        <v>106</v>
       </c>
       <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64" s="1">
-        <v>-0.3</v>
+        <v>7</v>
+      </c>
+      <c r="J64" t="s">
+        <v>124</v>
       </c>
       <c r="K64" t="s">
-        <v>26</v>
-      </c>
-      <c r="L64" s="5"/>
+        <v>144</v>
+      </c>
+      <c r="L64" s="4"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
       <c r="C65" t="s">
-        <v>16</v>
+        <v>78</v>
+      </c>
+      <c r="D65" t="s">
+        <v>106</v>
       </c>
       <c r="F65">
-        <v>-1</v>
-      </c>
-      <c r="G65" s="1">
-        <v>-0.25</v>
+        <v>7</v>
+      </c>
+      <c r="J65" t="s">
+        <v>124</v>
       </c>
       <c r="K65" t="s">
-        <v>18</v>
-      </c>
-      <c r="L65" s="5"/>
+        <v>143</v>
+      </c>
+      <c r="L65" s="4"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C66" t="s">
         <v>16</v>
@@ -2369,37 +2387,40 @@
         <v>-1</v>
       </c>
       <c r="G66" s="1">
-        <v>-0.35</v>
-      </c>
-      <c r="L66" s="5"/>
+        <v>-0.2</v>
+      </c>
+      <c r="K66" t="s">
+        <v>13</v>
+      </c>
+      <c r="L66" s="4"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s">
         <v>16</v>
       </c>
       <c r="F67">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="1">
         <v>-0.3</v>
       </c>
       <c r="K67" t="s">
-        <v>21</v>
-      </c>
-      <c r="L67" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="L67" s="4"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C68" t="s">
         <v>16</v>
@@ -2411,139 +2432,136 @@
         <v>-0.25</v>
       </c>
       <c r="K68" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="L68" s="4"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C69" t="s">
         <v>16</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G69" s="1">
-        <v>-0.25</v>
-      </c>
-      <c r="K69" t="s">
-        <v>25</v>
-      </c>
-      <c r="L69" s="5"/>
+        <v>-0.35</v>
+      </c>
+      <c r="L69" s="4"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C70" t="s">
         <v>16</v>
       </c>
       <c r="F70">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="G70" s="1">
-        <v>-0.25</v>
-      </c>
-      <c r="L70" s="5"/>
+        <v>-0.3</v>
+      </c>
+      <c r="K70" t="s">
+        <v>21</v>
+      </c>
+      <c r="L70" s="4"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>29</v>
-      </c>
-      <c r="H71">
-        <v>2</v>
-      </c>
-      <c r="I71" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="F71">
+        <v>-1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>-0.25</v>
       </c>
       <c r="K71" t="s">
-        <v>47</v>
-      </c>
-      <c r="L71" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="L71" s="4"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>29</v>
-      </c>
-      <c r="H72">
-        <v>1</v>
-      </c>
-      <c r="I72" t="s">
-        <v>45</v>
+        <v>16</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <v>-0.25</v>
       </c>
       <c r="K72" t="s">
-        <v>156</v>
-      </c>
-      <c r="L72" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="L72" s="4"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C73" t="s">
-        <v>29</v>
-      </c>
-      <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="I73" t="s">
-        <v>44</v>
-      </c>
-      <c r="K73" t="s">
-        <v>48</v>
-      </c>
-      <c r="L73" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="F73">
+        <v>-2</v>
+      </c>
+      <c r="G73" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="L73" s="4"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
       </c>
       <c r="H74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I74" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K74" t="s">
-        <v>49</v>
-      </c>
-      <c r="L74" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="L74" s="4"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>71</v>
       </c>
       <c r="B75" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C75" t="s">
         <v>29</v>
@@ -2552,82 +2570,82 @@
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K75" t="s">
-        <v>50</v>
-      </c>
-      <c r="L75" s="5"/>
+        <v>156</v>
+      </c>
+      <c r="L75" s="4"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>72</v>
       </c>
       <c r="B76" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C76" t="s">
         <v>29</v>
       </c>
       <c r="H76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K76" t="s">
-        <v>183</v>
-      </c>
-      <c r="L76" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="L76" s="4"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C77" t="s">
         <v>29</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I77" t="s">
         <v>45</v>
       </c>
       <c r="K77" t="s">
-        <v>51</v>
-      </c>
-      <c r="L77" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="L77" s="4"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C78" t="s">
         <v>29</v>
       </c>
       <c r="H78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I78" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K78" t="s">
-        <v>52</v>
-      </c>
-      <c r="L78" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="L78" s="4"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C79" t="s">
         <v>29</v>
@@ -2636,82 +2654,82 @@
         <v>2</v>
       </c>
       <c r="I79" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K79" t="s">
-        <v>53</v>
-      </c>
-      <c r="L79" s="5"/>
+        <v>183</v>
+      </c>
+      <c r="L79" s="4"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C80" t="s">
         <v>29</v>
       </c>
       <c r="H80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I80" t="s">
         <v>45</v>
       </c>
       <c r="K80" t="s">
-        <v>54</v>
-      </c>
-      <c r="L80" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="L80" s="4"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>77</v>
       </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C81" t="s">
         <v>29</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I81" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K81" t="s">
-        <v>55</v>
-      </c>
-      <c r="L81" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="L81" s="4"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C82" t="s">
         <v>29</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K82" t="s">
-        <v>56</v>
-      </c>
-      <c r="L82" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="L82" s="4"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C83" t="s">
         <v>29</v>
@@ -2723,30 +2741,93 @@
         <v>45</v>
       </c>
       <c r="K83" t="s">
-        <v>57</v>
-      </c>
-      <c r="L83" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="L83" s="4"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C84" t="s">
         <v>29</v>
       </c>
       <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>46</v>
+      </c>
+      <c r="K84" t="s">
+        <v>55</v>
+      </c>
+      <c r="L84" s="4"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>81</v>
+      </c>
+      <c r="B85" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85" t="s">
+        <v>46</v>
+      </c>
+      <c r="K85" t="s">
+        <v>56</v>
+      </c>
+      <c r="L85" s="4"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>82</v>
+      </c>
+      <c r="B86" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" t="s">
+        <v>29</v>
+      </c>
+      <c r="H86">
+        <v>2</v>
+      </c>
+      <c r="I86" t="s">
+        <v>45</v>
+      </c>
+      <c r="K86" t="s">
+        <v>57</v>
+      </c>
+      <c r="L86" s="4"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>83</v>
+      </c>
+      <c r="B87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" t="s">
+        <v>29</v>
+      </c>
+      <c r="H87">
         <v>3</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I87" t="s">
         <v>45</v>
       </c>
-      <c r="K84" t="s">
+      <c r="K87" t="s">
         <v>58</v>
       </c>
-      <c r="L84" s="5"/>
+      <c r="L87" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A5:N86">

</xml_diff>

<commit_message>
ADDED: Documents - Rulebook, card list, card sheets, card images of recent playtesting session.
</commit_message>
<xml_diff>
--- a/Documents/Card Lists/Card List - 01 Premiere.xlsx
+++ b/Documents/Card Lists/Card List - 01 Premiere.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="194">
   <si>
     <t>Card List - Premiere</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Every time an attack effect is played, remove (1).</t>
   </si>
   <si>
-    <t>Anaylze Attack</t>
-  </si>
-  <si>
     <t>MAIN: Reveal the top five cards of the attack deck. Remove (1) for each effect revealed. Return the cards in any order.</t>
   </si>
   <si>
@@ -584,6 +581,21 @@
   </si>
   <si>
     <t>MAIN: If your discard pile contains more cards than your draw deck, draw two cards.</t>
+  </si>
+  <si>
+    <t>Analyze Attack</t>
+  </si>
+  <si>
+    <t>Dra'tar Assault Cruiser</t>
+  </si>
+  <si>
+    <t>Dra'tar Assault Frigate</t>
+  </si>
+  <si>
+    <t>Dra'tar Behemoth</t>
+  </si>
+  <si>
+    <t>Dra'tar Swarm Frigate</t>
   </si>
 </sst>
 </file>
@@ -986,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
         <v>60</v>
@@ -1073,7 +1085,7 @@
         <v>61</v>
       </c>
       <c r="K5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L5" s="4"/>
     </row>
@@ -1082,7 +1094,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
         <v>60</v>
@@ -1091,7 +1103,7 @@
         <v>61</v>
       </c>
       <c r="K6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L6" s="4"/>
     </row>
@@ -1100,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
         <v>60</v>
@@ -1109,7 +1121,7 @@
         <v>61</v>
       </c>
       <c r="K7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L7" s="4"/>
     </row>
@@ -1118,7 +1130,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
         <v>60</v>
@@ -1127,7 +1139,7 @@
         <v>61</v>
       </c>
       <c r="K8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L8" s="4"/>
     </row>
@@ -1136,7 +1148,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
         <v>60</v>
@@ -1145,7 +1157,7 @@
         <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L9" s="4"/>
     </row>
@@ -1154,7 +1166,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
         <v>70</v>
@@ -1166,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L10" s="4"/>
     </row>
@@ -1175,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
         <v>70</v>
@@ -1187,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L11" s="4"/>
     </row>
@@ -1196,7 +1208,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
         <v>70</v>
@@ -1208,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L12" s="4"/>
     </row>
@@ -1217,7 +1229,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
         <v>70</v>
@@ -1229,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L13" s="4"/>
     </row>
@@ -1238,7 +1250,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C14" t="s">
         <v>70</v>
@@ -1250,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L14" s="4"/>
     </row>
@@ -1259,7 +1271,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
         <v>78</v>
@@ -1271,10 +1283,10 @@
         <v>8</v>
       </c>
       <c r="J15" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15" t="s">
         <v>139</v>
-      </c>
-      <c r="K15" t="s">
-        <v>140</v>
       </c>
       <c r="L15" s="4"/>
     </row>
@@ -1283,7 +1295,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
         <v>78</v>
@@ -1295,10 +1307,10 @@
         <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L16" s="4"/>
     </row>
@@ -1307,7 +1319,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
         <v>78</v>
@@ -1319,10 +1331,10 @@
         <v>8</v>
       </c>
       <c r="J17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L17" s="4"/>
     </row>
@@ -1331,7 +1343,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
         <v>78</v>
@@ -1343,10 +1355,10 @@
         <v>8</v>
       </c>
       <c r="J18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L18" s="4"/>
     </row>
@@ -1361,7 +1373,7 @@
         <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1382,13 +1394,13 @@
         <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L20" s="4"/>
     </row>
@@ -1403,7 +1415,7 @@
         <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1424,7 +1436,7 @@
         <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1445,7 +1457,7 @@
         <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1466,7 +1478,7 @@
         <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1487,7 +1499,7 @@
         <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1502,13 +1514,13 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E26">
         <v>5</v>
@@ -1529,13 +1541,13 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>190</v>
       </c>
       <c r="C27" t="s">
         <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -1553,13 +1565,13 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="C28" t="s">
         <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -1577,13 +1589,13 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C29" t="s">
         <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -1604,13 +1616,13 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>192</v>
       </c>
       <c r="C30" t="s">
         <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E30">
         <v>4</v>
@@ -1628,13 +1640,13 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C31" t="s">
         <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -1655,13 +1667,13 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C32" t="s">
         <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -1682,13 +1694,13 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C33" t="s">
         <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -1709,13 +1721,13 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C34" t="s">
         <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -1736,13 +1748,13 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C35" t="s">
         <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -1763,13 +1775,13 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>193</v>
       </c>
       <c r="C36" t="s">
         <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1796,10 +1808,10 @@
         <v>60</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L37" s="4"/>
     </row>
@@ -1814,7 +1826,7 @@
         <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K38" t="s">
         <v>63</v>
@@ -1832,10 +1844,10 @@
         <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L39" s="4"/>
     </row>
@@ -1850,7 +1862,7 @@
         <v>60</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K40" t="s">
         <v>66</v>
@@ -1868,10 +1880,10 @@
         <v>60</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L41" s="4"/>
     </row>
@@ -1886,10 +1898,10 @@
         <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L42" s="4"/>
     </row>
@@ -1904,13 +1916,13 @@
         <v>70</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L43" s="4"/>
     </row>
@@ -1925,13 +1937,13 @@
         <v>70</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="K44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L44" s="4"/>
     </row>
@@ -1940,19 +1952,19 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C45" t="s">
         <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="K45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L45" s="4"/>
     </row>
@@ -1967,13 +1979,13 @@
         <v>70</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L46" s="4"/>
     </row>
@@ -1988,13 +2000,13 @@
         <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="K47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L47" s="4"/>
     </row>
@@ -2009,7 +2021,7 @@
         <v>70</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E48">
         <v>3</v>
@@ -2030,7 +2042,7 @@
         <v>70</v>
       </c>
       <c r="D49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -2045,19 +2057,19 @@
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C50" t="s">
         <v>78</v>
       </c>
       <c r="D50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F50">
         <v>7</v>
       </c>
       <c r="J50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K50" t="s">
         <v>79</v>
@@ -2069,22 +2081,22 @@
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C51" t="s">
         <v>78</v>
       </c>
       <c r="D51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F51">
         <v>7</v>
       </c>
       <c r="J51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L51" s="4"/>
     </row>
@@ -2138,7 +2150,7 @@
         <v>106</v>
       </c>
       <c r="K54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L54" s="4"/>
     </row>
@@ -2183,7 +2195,7 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>189</v>
       </c>
       <c r="C57" t="s">
         <v>70</v>
@@ -2195,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="K57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L57" s="4"/>
     </row>
@@ -2204,7 +2216,7 @@
         <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58" t="s">
         <v>70</v>
@@ -2216,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="K58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L58" s="4"/>
     </row>
@@ -2225,7 +2237,7 @@
         <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C59" t="s">
         <v>70</v>
@@ -2237,7 +2249,7 @@
         <v>0</v>
       </c>
       <c r="K59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L59" s="4"/>
     </row>
@@ -2246,7 +2258,7 @@
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C60" t="s">
         <v>70</v>
@@ -2258,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="K60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L60" s="4"/>
     </row>
@@ -2267,7 +2279,7 @@
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s">
         <v>70</v>
@@ -2279,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="K61" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L61" s="4"/>
     </row>
@@ -2288,7 +2300,7 @@
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" t="s">
         <v>70</v>
@@ -2300,7 +2312,7 @@
         <v>2</v>
       </c>
       <c r="K62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L62" s="4"/>
     </row>
@@ -2309,7 +2321,7 @@
         <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C63" t="s">
         <v>70</v>
@@ -2321,7 +2333,7 @@
         <v>1</v>
       </c>
       <c r="K63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L63" s="4"/>
     </row>
@@ -2330,7 +2342,7 @@
         <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C64" t="s">
         <v>78</v>
@@ -2342,10 +2354,10 @@
         <v>7</v>
       </c>
       <c r="J64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L64" s="4"/>
     </row>
@@ -2354,7 +2366,7 @@
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C65" t="s">
         <v>78</v>
@@ -2366,10 +2378,10 @@
         <v>7</v>
       </c>
       <c r="J65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L65" s="4"/>
     </row>
@@ -2573,7 +2585,7 @@
         <v>45</v>
       </c>
       <c r="K75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L75" s="4"/>
     </row>
@@ -2657,7 +2669,7 @@
         <v>46</v>
       </c>
       <c r="K79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L79" s="4"/>
     </row>

</xml_diff>